<commit_message>
Downloaded and tried on new data
</commit_message>
<xml_diff>
--- a/Inputs/flipAPDV.xlsx
+++ b/Inputs/flipAPDV.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\QualitativeAnalysisCalciumWaves\Quantitative\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsoundar\Documents\GitHub\intercellular_calcium_wave_toolkit\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A88E17C-EF4F-41C3-805F-2BBE368A8653}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="2820" windowWidth="28800" windowHeight="16455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2325" yWindow="2820" windowWidth="28800" windowHeight="16455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="90">
   <si>
     <t>Label</t>
   </si>
@@ -266,12 +265,36 @@
   </si>
   <si>
     <t>3_17_2018 1346 x 428 tkv-ca Sample 6</t>
+  </si>
+  <si>
+    <t>11.6.18.1.1</t>
+  </si>
+  <si>
+    <t>11.6.18.1.2</t>
+  </si>
+  <si>
+    <t>11.6.18.2.1</t>
+  </si>
+  <si>
+    <t>11.6.18.2.2</t>
+  </si>
+  <si>
+    <t>11.6.18.2.3</t>
+  </si>
+  <si>
+    <t>11.6.18.3.1</t>
+  </si>
+  <si>
+    <t>11.6.18.3.2</t>
+  </si>
+  <si>
+    <t>11.6.18.3.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,7 +405,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -694,11 +717,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:J68"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,6 +2919,262 @@
         <v>67</v>
       </c>
     </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" t="s">
+        <v>64</v>
+      </c>
+      <c r="F69" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" t="s">
+        <v>9</v>
+      </c>
+      <c r="H69" t="s">
+        <v>9</v>
+      </c>
+      <c r="I69" t="s">
+        <v>9</v>
+      </c>
+      <c r="J69" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" t="s">
+        <v>64</v>
+      </c>
+      <c r="F70" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70" t="s">
+        <v>9</v>
+      </c>
+      <c r="H70" t="s">
+        <v>9</v>
+      </c>
+      <c r="I70" t="s">
+        <v>9</v>
+      </c>
+      <c r="J70" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" t="s">
+        <v>65</v>
+      </c>
+      <c r="E71" t="s">
+        <v>65</v>
+      </c>
+      <c r="F71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" t="s">
+        <v>9</v>
+      </c>
+      <c r="H71" t="s">
+        <v>9</v>
+      </c>
+      <c r="I71" t="s">
+        <v>9</v>
+      </c>
+      <c r="J71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" t="s">
+        <v>67</v>
+      </c>
+      <c r="E72" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>9</v>
+      </c>
+      <c r="H72" t="s">
+        <v>9</v>
+      </c>
+      <c r="I72" t="s">
+        <v>9</v>
+      </c>
+      <c r="J72" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73" t="s">
+        <v>67</v>
+      </c>
+      <c r="C73" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" t="s">
+        <v>67</v>
+      </c>
+      <c r="E73" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" t="s">
+        <v>9</v>
+      </c>
+      <c r="H73" t="s">
+        <v>9</v>
+      </c>
+      <c r="I73" t="s">
+        <v>9</v>
+      </c>
+      <c r="J73" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" t="s">
+        <v>64</v>
+      </c>
+      <c r="D74" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" t="s">
+        <v>64</v>
+      </c>
+      <c r="F74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" t="s">
+        <v>9</v>
+      </c>
+      <c r="H74" t="s">
+        <v>9</v>
+      </c>
+      <c r="I74" t="s">
+        <v>9</v>
+      </c>
+      <c r="J74" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" t="s">
+        <v>64</v>
+      </c>
+      <c r="D75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" t="s">
+        <v>64</v>
+      </c>
+      <c r="F75" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" t="s">
+        <v>9</v>
+      </c>
+      <c r="H75" t="s">
+        <v>9</v>
+      </c>
+      <c r="I75" t="s">
+        <v>9</v>
+      </c>
+      <c r="J75" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" t="s">
+        <v>64</v>
+      </c>
+      <c r="D76" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" t="s">
+        <v>64</v>
+      </c>
+      <c r="F76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" t="s">
+        <v>9</v>
+      </c>
+      <c r="H76" t="s">
+        <v>9</v>
+      </c>
+      <c r="I76" t="s">
+        <v>9</v>
+      </c>
+      <c r="J76" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:J54">
     <sortCondition ref="A1"/>

</xml_diff>